<commit_message>
big update of pre-defined pdfs from google docs, everything in place now except cover, need to finalize preface
</commit_message>
<xml_diff>
--- a/data/completePaperList.xlsx
+++ b/data/completePaperList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="paperList.txt" sheetId="1" state="visible" r:id="rId2"/>
@@ -3945,15 +3945,15 @@
   </sheetPr>
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5562,7 +5562,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10351,13 +10351,16 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.21395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5023255813953"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10368,7 +10371,7 @@
         <v>1237</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10390,7 +10393,7 @@
         <v>1239</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10401,7 +10404,7 @@
         <v>1240</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10412,7 +10415,7 @@
         <v>1241</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10423,7 +10426,7 @@
         <v>1242</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10434,7 +10437,7 @@
         <v>1243</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10445,7 +10448,7 @@
         <v>1244</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10494,7 +10497,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10927,7 +10930,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11374,7 +11377,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.05116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated session index and corresponding spreadsheet page to reflect new front mater
</commit_message>
<xml_diff>
--- a/data/completePaperList.xlsx
+++ b/data/completePaperList.xlsx
@@ -13,7 +13,7 @@
     <sheet name="programCommittee" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="reviewersFirstLastSeparate" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="sessions" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="sessionsManualPages" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="session_index" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="posters1sorted" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="posters2sorted" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="posters3sorted" sheetId="9" state="visible" r:id="rId10"/>
@@ -12872,7 +12872,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12899,7 +12899,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>1525</v>
@@ -12910,7 +12910,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>1526</v>
@@ -12921,7 +12921,7 @@
         <v>70</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>1527</v>
@@ -12932,7 +12932,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>1528</v>
@@ -12943,7 +12943,7 @@
         <v>86</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>1529</v>
@@ -12954,7 +12954,7 @@
         <v>147</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>1530</v>
@@ -12965,7 +12965,7 @@
         <v>156</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>1531</v>
@@ -12976,7 +12976,7 @@
         <v>163</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>1532</v>
@@ -12987,7 +12987,7 @@
         <v>222</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>1533</v>
@@ -12998,7 +12998,7 @@
         <v>231</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>1534</v>

</xml_diff>